<commit_message>
using ordinal attribute values to calculate Moran's I
</commit_message>
<xml_diff>
--- a/surveyResults/Results2sheets.xlsx
+++ b/surveyResults/Results2sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\choroColorRead\surveyResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1628F8E-7253-4ECB-BF2D-6A0107534370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E209303F-8173-45E3-8360-17F39220D90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2278,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3166,6 +3166,18 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="C16">
+        <f>SUM(C2:C15)</f>
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:E16" si="3">SUM(D2:D15)</f>
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -4047,142 +4059,176 @@
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31">
-        <f>SUM(C2:C30)</f>
-        <v>47</v>
-      </c>
-      <c r="D31">
-        <f t="shared" ref="D31:W31" si="3">SUM(D2:D30)</f>
-        <v>126</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="3"/>
-        <v>161</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="3"/>
-        <v>71</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="3"/>
-        <v>146</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="3"/>
-        <v>301</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="3"/>
-        <v>255</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="W31">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="Y31">
-        <f>SUM(C31:W31)</f>
-        <v>1328</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
+        <f>SUM(C17:C30)</f>
+        <v>20</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" ref="D31:E31" si="4">SUM(D17:D30)</f>
+        <v>63</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <f>SUM(C2:C30)</f>
+        <v>74</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32:W32" si="5">SUM(D2:D30)</f>
+        <v>189</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="5"/>
+        <v>242</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>146</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="5"/>
+        <v>301</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="Y32">
+        <f>SUM(C32:W32)</f>
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
         <v>12</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>19</v>
       </c>
-      <c r="E32">
-        <v>5</v>
-      </c>
-      <c r="I32" s="2">
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="I33" s="2">
         <v>10</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J33" s="2">
         <v>11</v>
       </c>
-      <c r="K32" s="2">
-        <v>3</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="O32" s="2">
+      <c r="K33" s="2">
+        <v>3</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="O33" s="2">
         <v>20</v>
       </c>
-      <c r="P32" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="2">
+      <c r="P33" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="2">
         <v>4</v>
       </c>
-      <c r="S32">
+      <c r="S33">
         <v>14</v>
       </c>
-      <c r="U32" s="2">
+      <c r="U33" s="2">
         <v>14</v>
       </c>
-      <c r="V32" s="2">
-        <v>5</v>
-      </c>
-      <c r="W32" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
-        <v>2</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33" s="2">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2">
-        <v>2</v>
-      </c>
-      <c r="K33" s="2">
-        <v>0</v>
-      </c>
-      <c r="O33" s="2">
-        <v>1</v>
-      </c>
-      <c r="P33" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>0</v>
-      </c>
-      <c r="R33">
+      <c r="V33" s="2">
+        <v>5</v>
+      </c>
+      <c r="W33" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1</v>
+      </c>
+      <c r="J34" s="2">
+        <v>2</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2">
+        <v>1</v>
+      </c>
+      <c r="P34" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>0</v>
+      </c>
+      <c r="R34">
         <f>16*83</f>
         <v>1328</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B35" t="s">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>